<commit_message>
Added calibration to sensor data.
</commit_message>
<xml_diff>
--- a/calibration_work/Sensor_Testing_Data/Chase_Beth_Testing_12_05_2017.xlsx
+++ b/calibration_work/Sensor_Testing_Data/Chase_Beth_Testing_12_05_2017.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28315"/>
+  <workbookPr filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kreitzem/code/github/dean_lab/HaybaleSensor/calibration_work/Sensor_Testing_Data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="12 May 17" sheetId="1" r:id="rId1"/>
@@ -13,9 +18,15 @@
     <sheet name="16 May 17 Graphs" sheetId="4" r:id="rId4"/>
     <sheet name="Combined Data For all Days" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -23,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="23">
   <si>
     <t>Beth and Chase Measurements with Yellow Meter and Four Probes</t>
   </si>
@@ -87,12 +98,18 @@
   <si>
     <t>HB4</t>
   </si>
+  <si>
+    <t>HB7</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,6 +125,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -130,7 +153,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -145,6 +168,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -163,7 +187,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -272,31 +296,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>16293</c:v>
+                  <c:v>16293.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13109</c:v>
+                  <c:v>13109.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16319</c:v>
+                  <c:v>16319.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16155</c:v>
+                  <c:v>16155.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12854</c:v>
+                  <c:v>12854.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14906</c:v>
+                  <c:v>14906.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>16267</c:v>
+                  <c:v>16267.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16305</c:v>
+                  <c:v>16305.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>14615</c:v>
+                  <c:v>14615.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -308,13 +332,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>72.900000000000006</c:v>
+                  <c:v>72.9</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>83.1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>70</c:v>
+                  <c:v>70.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>79.3</c:v>
@@ -329,16 +353,16 @@
                   <c:v>79.2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>74.900000000000006</c:v>
+                  <c:v>74.9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>90</c:v>
+                  <c:v>90.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-5F7C-4763-9713-656E8FC09D65}"/>
             </c:ext>
@@ -379,31 +403,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>16229</c:v>
+                  <c:v>16229.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15264</c:v>
+                  <c:v>15264.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15927</c:v>
+                  <c:v>15927.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16629</c:v>
+                  <c:v>16629.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8296</c:v>
+                  <c:v>8296.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14413</c:v>
+                  <c:v>14413.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>16162</c:v>
+                  <c:v>16162.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>15465</c:v>
+                  <c:v>15465.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>14079</c:v>
+                  <c:v>14079.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -415,13 +439,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>72.900000000000006</c:v>
+                  <c:v>72.9</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>83.1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>70</c:v>
+                  <c:v>70.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>79.3</c:v>
@@ -436,16 +460,16 @@
                   <c:v>79.2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>74.900000000000006</c:v>
+                  <c:v>74.9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>90</c:v>
+                  <c:v>90.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-5F7C-4763-9713-656E8FC09D65}"/>
             </c:ext>
@@ -486,31 +510,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>16198</c:v>
+                  <c:v>16198.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15236</c:v>
+                  <c:v>15236.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16230</c:v>
+                  <c:v>16230.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15910</c:v>
+                  <c:v>15910.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11012</c:v>
+                  <c:v>11012.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13574</c:v>
+                  <c:v>13574.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>16345</c:v>
+                  <c:v>16345.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>15842</c:v>
+                  <c:v>15842.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>12666</c:v>
+                  <c:v>12666.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -522,13 +546,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>72.900000000000006</c:v>
+                  <c:v>72.9</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>83.1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>70</c:v>
+                  <c:v>70.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>79.3</c:v>
@@ -543,16 +567,16 @@
                   <c:v>79.2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>74.900000000000006</c:v>
+                  <c:v>74.9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>90</c:v>
+                  <c:v>90.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-5F7C-4763-9713-656E8FC09D65}"/>
             </c:ext>
@@ -593,31 +617,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>14834</c:v>
+                  <c:v>14834.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8642</c:v>
+                  <c:v>8642.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15410</c:v>
+                  <c:v>15410.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10933</c:v>
+                  <c:v>10933.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6812</c:v>
+                  <c:v>6812.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7148</c:v>
+                  <c:v>7148.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>14342</c:v>
+                  <c:v>14342.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>13546</c:v>
+                  <c:v>13546.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6771</c:v>
+                  <c:v>6771.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -629,13 +653,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>72.900000000000006</c:v>
+                  <c:v>72.9</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>83.1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>70</c:v>
+                  <c:v>70.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>79.3</c:v>
@@ -650,16 +674,16 @@
                   <c:v>79.2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>74.900000000000006</c:v>
+                  <c:v>74.9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>90</c:v>
+                  <c:v>90.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-5F7C-4763-9713-656E8FC09D65}"/>
             </c:ext>
@@ -673,14 +697,14 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="242151608"/>
-        <c:axId val="242150296"/>
+        <c:axId val="-579214384"/>
+        <c:axId val="-580081392"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="242151608"/>
+        <c:axId val="-579214384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="6000"/>
+          <c:min val="6000.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -790,12 +814,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="242150296"/>
+        <c:crossAx val="-580081392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="242150296"/>
+        <c:axId val="-580081392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -907,7 +931,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="242151608"/>
+        <c:crossAx val="-579214384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -988,7 +1012,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1097,31 +1121,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>4310</c:v>
+                  <c:v>4310.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4310</c:v>
+                  <c:v>4310.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4366</c:v>
+                  <c:v>4366.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4386</c:v>
+                  <c:v>4386.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4310</c:v>
+                  <c:v>4310.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4464</c:v>
+                  <c:v>4464.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4484</c:v>
+                  <c:v>4484.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4505</c:v>
+                  <c:v>4505.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4608</c:v>
+                  <c:v>4608.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1163,7 +1187,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-34EC-4A67-99DC-22E2405EDA35}"/>
             </c:ext>
@@ -1204,31 +1228,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>4464</c:v>
+                  <c:v>4464.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4385</c:v>
+                  <c:v>4385.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4386</c:v>
+                  <c:v>4386.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4292</c:v>
+                  <c:v>4292.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4273</c:v>
+                  <c:v>4273.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4329</c:v>
+                  <c:v>4329.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4405</c:v>
+                  <c:v>4405.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4405</c:v>
+                  <c:v>4405.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4504</c:v>
+                  <c:v>4504.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1270,7 +1294,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-34EC-4A67-99DC-22E2405EDA35}"/>
             </c:ext>
@@ -1311,31 +1335,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>4405</c:v>
+                  <c:v>4405.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4545</c:v>
+                  <c:v>4545.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4587</c:v>
+                  <c:v>4587.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4504</c:v>
+                  <c:v>4504.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4464</c:v>
+                  <c:v>4464.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4545</c:v>
+                  <c:v>4545.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4629</c:v>
+                  <c:v>4629.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4587</c:v>
+                  <c:v>4587.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4695</c:v>
+                  <c:v>4695.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1377,7 +1401,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-34EC-4A67-99DC-22E2405EDA35}"/>
             </c:ext>
@@ -1418,31 +1442,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>4504</c:v>
+                  <c:v>4504.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4464</c:v>
+                  <c:v>4464.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4504</c:v>
+                  <c:v>4504.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4405</c:v>
+                  <c:v>4405.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4444</c:v>
+                  <c:v>4444.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4566</c:v>
+                  <c:v>4566.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4545</c:v>
+                  <c:v>4545.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4545</c:v>
+                  <c:v>4545.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4695</c:v>
+                  <c:v>4695.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1484,7 +1508,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-34EC-4A67-99DC-22E2405EDA35}"/>
             </c:ext>
@@ -1498,11 +1522,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="243455344"/>
-        <c:axId val="243461904"/>
+        <c:axId val="-459212896"/>
+        <c:axId val="-459208624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="243455344"/>
+        <c:axId val="-459212896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1614,12 +1638,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="243461904"/>
+        <c:crossAx val="-459208624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="243461904"/>
+        <c:axId val="-459208624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1731,7 +1755,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="243455344"/>
+        <c:crossAx val="-459212896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1812,7 +1836,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1896,34 +1920,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>16387</c:v>
+                  <c:v>16387.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13081</c:v>
+                  <c:v>13081.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13269</c:v>
+                  <c:v>13269.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15865</c:v>
+                  <c:v>15865.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12672</c:v>
+                  <c:v>12672.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14647</c:v>
+                  <c:v>14647.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>16162</c:v>
+                  <c:v>16162.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16194</c:v>
+                  <c:v>16194.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>16127</c:v>
+                  <c:v>16127.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>15137</c:v>
+                  <c:v>15137.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1944,7 +1968,7 @@
                   <c:v>94.3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>80.599999999999994</c:v>
+                  <c:v>80.6</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>84.7</c:v>
@@ -1953,7 +1977,7 @@
                   <c:v>84.7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>85</c:v>
+                  <c:v>85.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>60.5</c:v>
@@ -1968,7 +1992,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-C092-4479-BC4C-7B3D6590CD0A}"/>
             </c:ext>
@@ -2009,34 +2033,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>16332</c:v>
+                  <c:v>16332.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14754</c:v>
+                  <c:v>14754.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13434</c:v>
+                  <c:v>13434.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16057</c:v>
+                  <c:v>16057.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11711</c:v>
+                  <c:v>11711.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11503</c:v>
+                  <c:v>11503.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11902</c:v>
+                  <c:v>11902.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16179</c:v>
+                  <c:v>16179.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>15685</c:v>
+                  <c:v>15685.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>15781</c:v>
+                  <c:v>15781.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2057,7 +2081,7 @@
                   <c:v>94.3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>80.599999999999994</c:v>
+                  <c:v>80.6</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>84.7</c:v>
@@ -2066,7 +2090,7 @@
                   <c:v>84.7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>85</c:v>
+                  <c:v>85.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>60.5</c:v>
@@ -2081,7 +2105,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-C092-4479-BC4C-7B3D6590CD0A}"/>
             </c:ext>
@@ -2122,34 +2146,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>16499</c:v>
+                  <c:v>16499.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15783</c:v>
+                  <c:v>15783.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12715</c:v>
+                  <c:v>12715.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16304</c:v>
+                  <c:v>16304.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14409</c:v>
+                  <c:v>14409.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16075</c:v>
+                  <c:v>16075.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>14960</c:v>
+                  <c:v>14960.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16301</c:v>
+                  <c:v>16301.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>16320</c:v>
+                  <c:v>16320.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>14960</c:v>
+                  <c:v>14960.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2170,7 +2194,7 @@
                   <c:v>94.3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>80.599999999999994</c:v>
+                  <c:v>80.6</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>84.7</c:v>
@@ -2179,7 +2203,7 @@
                   <c:v>84.7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>85</c:v>
+                  <c:v>85.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>60.5</c:v>
@@ -2194,7 +2218,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-C092-4479-BC4C-7B3D6590CD0A}"/>
             </c:ext>
@@ -2208,14 +2232,14 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="314418848"/>
-        <c:axId val="314420160"/>
+        <c:axId val="-579174016"/>
+        <c:axId val="-579170256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="314418848"/>
+        <c:axId val="-579174016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="10000"/>
+          <c:min val="10000.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -2300,12 +2324,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="314420160"/>
+        <c:crossAx val="-579170256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="314420160"/>
+        <c:axId val="-579170256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2392,7 +2416,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="314418848"/>
+        <c:crossAx val="-579174016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2473,7 +2497,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2557,34 +2581,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>4608</c:v>
+                  <c:v>4608.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4587</c:v>
+                  <c:v>4587.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4630</c:v>
+                  <c:v>4630.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4673</c:v>
+                  <c:v>4673.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4717</c:v>
+                  <c:v>4717.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4673</c:v>
+                  <c:v>4673.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4902</c:v>
+                  <c:v>4902.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4926</c:v>
+                  <c:v>4926.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4831</c:v>
+                  <c:v>4831.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4854</c:v>
+                  <c:v>4854.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2617,7 +2641,7 @@
                   <c:v>24.6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>26</c:v>
+                  <c:v>26.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>25.3</c:v>
@@ -2629,7 +2653,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000008-6A9C-4BFF-9F5B-F16E49461D6B}"/>
             </c:ext>
@@ -2670,34 +2694,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>4525</c:v>
+                  <c:v>4525.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4630</c:v>
+                  <c:v>4630.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4673</c:v>
+                  <c:v>4673.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4630</c:v>
+                  <c:v>4630.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4673</c:v>
+                  <c:v>4673.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4630</c:v>
+                  <c:v>4630.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4808</c:v>
+                  <c:v>4808.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4878</c:v>
+                  <c:v>4878.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4831</c:v>
+                  <c:v>4831.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4951</c:v>
+                  <c:v>4951.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2730,7 +2754,7 @@
                   <c:v>24.6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>26</c:v>
+                  <c:v>26.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>25.3</c:v>
@@ -2742,7 +2766,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000009-6A9C-4BFF-9F5B-F16E49461D6B}"/>
             </c:ext>
@@ -2783,34 +2807,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>4587</c:v>
+                  <c:v>4587.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4739</c:v>
+                  <c:v>4739.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4739</c:v>
+                  <c:v>4739.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4785</c:v>
+                  <c:v>4785.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4831</c:v>
+                  <c:v>4831.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5051</c:v>
+                  <c:v>5051.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5000</c:v>
+                  <c:v>5000.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5050</c:v>
+                  <c:v>5050.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5051</c:v>
+                  <c:v>5051.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5051</c:v>
+                  <c:v>5051.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2843,7 +2867,7 @@
                   <c:v>24.6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>26</c:v>
+                  <c:v>26.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>25.3</c:v>
@@ -2855,7 +2879,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000A-6A9C-4BFF-9F5B-F16E49461D6B}"/>
             </c:ext>
@@ -2869,11 +2893,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="407021920"/>
-        <c:axId val="408051280"/>
+        <c:axId val="-579137792"/>
+        <c:axId val="-579134032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="407021920"/>
+        <c:axId val="-579137792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2960,12 +2984,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="408051280"/>
+        <c:crossAx val="-579134032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="408051280"/>
+        <c:axId val="-579134032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3052,7 +3076,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="407021920"/>
+        <c:crossAx val="-579137792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3133,7 +3157,7 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3172,6 +3196,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3208,10 +3233,132 @@
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="3"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>HB2</c:v>
+            <c:v>HB7 Calibration</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.0884618758098275"/>
+                  <c:y val="0.144445538057743"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Combined Data For all Days'!$O$21:$O$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>16703.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7172.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7426.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6346.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Combined Data For all Days'!$N$21:$N$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Sensor Data</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -3235,86 +3382,106 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.105992424997508"/>
+                  <c:y val="0.255599664625255"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Combined Data For all Days'!$E$4:$E$22</c:f>
+              <c:f>'Combined Data For all Days'!$E$61:$E$69</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>16293</c:v>
+                  <c:v>14834.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13109</c:v>
+                  <c:v>8642.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16319</c:v>
+                  <c:v>15410.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16155</c:v>
+                  <c:v>10933.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12854</c:v>
+                  <c:v>6812.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14906</c:v>
+                  <c:v>7148.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>16267</c:v>
+                  <c:v>14342.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16305</c:v>
+                  <c:v>13546.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>14615</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>16387</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>13081</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>13269</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>15865</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>12672</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>14647</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16162</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>16194</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>16127</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>15137</c:v>
+                  <c:v>6771.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Combined Data For all Days'!$C$4:$C$22</c:f>
+              <c:f>'Combined Data For all Days'!$C$61:$C$69</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>72.900000000000006</c:v>
+                  <c:v>72.9</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>83.1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>70</c:v>
+                  <c:v>70.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>79.3</c:v>
@@ -3329,384 +3496,15 @@
                   <c:v>79.2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>74.900000000000006</c:v>
+                  <c:v>74.9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>71.5</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>84.8</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>94.3</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>80.599999999999994</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>84.7</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>84.7</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>85</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>60.5</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>65.7</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>87.8</c:v>
+                  <c:v>90.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-4141-4F4D-B7D1-23A16A0F5100}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>HB4</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Combined Data For all Days'!$E$23:$E$41</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>16229</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>15264</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>15927</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>16629</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8296</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>14413</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>16162</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>15465</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>14079</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>16332</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>14754</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>13434</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>16057</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>11711</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>11503</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>11902</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>16179</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>15685</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>15781</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Combined Data For all Days'!$C$23:$C$41</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>72.900000000000006</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>83.1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>79.3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>92.5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>87.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>79.2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>74.900000000000006</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>71.5</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>84.8</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>94.3</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>80.599999999999994</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>84.7</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>84.7</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>85</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>60.5</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>65.7</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>87.8</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-4141-4F4D-B7D1-23A16A0F5100}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>HB6</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Combined Data For all Days'!$E$42:$E$60</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>16198</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>15236</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>16230</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>15910</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>11012</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>13574</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>16345</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>15842</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>12666</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>16499</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>15783</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12715</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>16304</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14409</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>16075</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>14960</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>16301</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>16320</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>14960</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Combined Data For all Days'!$C$42:$C$60</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>72.900000000000006</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>83.1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>79.3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>92.5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>87.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>79.2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>74.900000000000006</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>71.5</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>84.8</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>94.3</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>80.599999999999994</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>84.7</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>84.7</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>85</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>60.5</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>65.7</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>87.8</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-4141-4F4D-B7D1-23A16A0F5100}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -3716,14 +3514,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="408634312"/>
-        <c:axId val="407021920"/>
+        <c:axId val="-579090368"/>
+        <c:axId val="-579086608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="408634312"/>
+        <c:axId val="-579090368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="8000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -3742,6 +3539,7 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3808,12 +3606,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="407021920"/>
+        <c:crossAx val="-579086608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="407021920"/>
+        <c:axId val="-579086608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3834,6 +3632,7 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3900,7 +3699,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="408634312"/>
+        <c:crossAx val="-579090368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3914,6 +3713,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6780,7 +6580,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DD071F8-CCC0-4E7C-8DC7-AEA10750F3AE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9DD071F8-CCC0-4E7C-8DC7-AEA10750F3AE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6816,7 +6616,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1D7C355-1D04-4992-965B-AECBB36E2101}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A1D7C355-1D04-4992-965B-AECBB36E2101}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6857,7 +6657,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{408ED6C3-DEFE-447F-8E19-4B566CF5E695}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{408ED6C3-DEFE-447F-8E19-4B566CF5E695}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6893,7 +6693,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8333890C-53D9-4B5C-8BFE-13E2D523CC64}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8333890C-53D9-4B5C-8BFE-13E2D523CC64}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6934,7 +6734,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A72EA52-14BE-4D46-9B66-752942A9DC70}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0A72EA52-14BE-4D46-9B66-752942A9DC70}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7258,22 +7058,22 @@
       <selection sqref="A1:H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" style="4" customWidth="1"/>
-    <col min="3" max="5" width="9.140625" style="4"/>
+    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" style="4" customWidth="1"/>
+    <col min="3" max="5" width="8.83203125" style="4"/>
     <col min="6" max="6" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="4"/>
+    <col min="7" max="7" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1">
         <v>42867</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -7281,7 +7081,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -7293,7 +7093,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
         <v>13</v>
       </c>
@@ -7313,7 +7113,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -7336,7 +7136,7 @@
         <v>3.83</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -7359,7 +7159,7 @@
         <v>4.26</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -7382,7 +7182,7 @@
         <v>3.74</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -7405,7 +7205,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -7428,7 +7228,7 @@
         <v>3.84</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -7451,7 +7251,7 @@
         <v>3.71</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -7474,7 +7274,7 @@
         <v>4.2699999999999996</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -7497,7 +7297,7 @@
         <v>4.0199999999999996</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -7520,7 +7320,7 @@
         <v>3.82</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -7543,7 +7343,7 @@
         <v>3.72</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -7566,7 +7366,7 @@
         <v>4.2699999999999996</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -7589,7 +7389,7 @@
         <v>4.0199999999999996</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -7612,7 +7412,7 @@
         <v>3.82</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -7635,7 +7435,7 @@
         <v>3.72</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -7658,7 +7458,7 @@
         <v>4.26</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -7681,7 +7481,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -7704,7 +7504,7 @@
         <v>3.83</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -7727,7 +7527,7 @@
         <v>3.72</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>11</v>
       </c>
@@ -7750,7 +7550,7 @@
         <v>4.26</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -7773,7 +7573,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -7796,7 +7596,7 @@
         <v>3.84</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -7819,7 +7619,7 @@
         <v>3.72</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>11</v>
       </c>
@@ -7842,7 +7642,7 @@
         <v>4.26</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>12</v>
       </c>
@@ -7865,7 +7665,7 @@
         <v>4.01</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>9</v>
       </c>
@@ -7888,7 +7688,7 @@
         <v>3.84</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>10</v>
       </c>
@@ -7911,7 +7711,7 @@
         <v>3.72</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>11</v>
       </c>
@@ -7934,7 +7734,7 @@
         <v>4.26</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>12</v>
       </c>
@@ -7957,7 +7757,7 @@
         <v>3.99</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>9</v>
       </c>
@@ -7980,7 +7780,7 @@
         <v>3.83</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>10</v>
       </c>
@@ -8003,7 +7803,7 @@
         <v>3.72</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>11</v>
       </c>
@@ -8026,7 +7826,7 @@
         <v>4.3600000000000003</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>12</v>
       </c>
@@ -8049,7 +7849,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>9</v>
       </c>
@@ -8072,7 +7872,7 @@
         <v>3.85</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>10</v>
       </c>
@@ -8095,7 +7895,7 @@
         <v>3.73</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>11</v>
       </c>
@@ -8118,7 +7918,7 @@
         <v>4.26</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>12</v>
       </c>
@@ -8155,12 +7955,12 @@
       <selection activeCell="A6" sqref="A6:G41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -8178,7 +7978,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
         <v>13</v>
       </c>
@@ -8204,7 +8004,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -8233,7 +8033,7 @@
         <v>0.28639999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -8256,7 +8056,7 @@
         <v>3.84</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -8279,7 +8079,7 @@
         <v>3.82</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -8302,7 +8102,7 @@
         <v>3.82</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -8325,7 +8125,7 @@
         <v>3.83</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -8348,7 +8148,7 @@
         <v>3.84</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -8371,7 +8171,7 @@
         <v>3.84</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -8394,7 +8194,7 @@
         <v>3.83</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -8417,7 +8217,7 @@
         <v>3.85</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -8446,7 +8246,7 @@
         <v>0.33560000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -8469,7 +8269,7 @@
         <v>3.71</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -8492,7 +8292,7 @@
         <v>3.72</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -8515,7 +8315,7 @@
         <v>3.72</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -8538,7 +8338,7 @@
         <v>3.72</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -8561,7 +8361,7 @@
         <v>3.72</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -8584,7 +8384,7 @@
         <v>3.72</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>10</v>
       </c>
@@ -8607,7 +8407,7 @@
         <v>3.72</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -8630,7 +8430,7 @@
         <v>3.73</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>11</v>
       </c>
@@ -8659,7 +8459,7 @@
         <v>2.9499999999999998E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>11</v>
       </c>
@@ -8682,7 +8482,7 @@
         <v>4.2699999999999996</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>11</v>
       </c>
@@ -8705,7 +8505,7 @@
         <v>4.2699999999999996</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>11</v>
       </c>
@@ -8728,7 +8528,7 @@
         <v>4.26</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>11</v>
       </c>
@@ -8751,7 +8551,7 @@
         <v>4.26</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>11</v>
       </c>
@@ -8774,7 +8574,7 @@
         <v>4.26</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>11</v>
       </c>
@@ -8797,7 +8597,7 @@
         <v>4.26</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>11</v>
       </c>
@@ -8820,7 +8620,7 @@
         <v>4.3600000000000003</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>11</v>
       </c>
@@ -8843,7 +8643,7 @@
         <v>4.26</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>12</v>
       </c>
@@ -8872,7 +8672,7 @@
         <v>0.46679999999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>12</v>
       </c>
@@ -8895,7 +8695,7 @@
         <v>4.0199999999999996</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>12</v>
       </c>
@@ -8918,7 +8718,7 @@
         <v>4.0199999999999996</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>12</v>
       </c>
@@ -8941,7 +8741,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>12</v>
       </c>
@@ -8964,7 +8764,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>12</v>
       </c>
@@ -8987,7 +8787,7 @@
         <v>4.01</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>12</v>
       </c>
@@ -9010,7 +8810,7 @@
         <v>3.99</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>12</v>
       </c>
@@ -9033,7 +8833,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>12</v>
       </c>
@@ -9069,23 +8869,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="9.140625" style="4"/>
+    <col min="1" max="1" width="10.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1">
         <v>42871</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -9093,10 +8893,10 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -9108,7 +8908,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5"/>
       <c r="B5" s="4" t="s">
         <v>13</v>
@@ -9129,7 +8929,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>18</v>
       </c>
@@ -9152,7 +8952,7 @@
         <v>3.83</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>19</v>
       </c>
@@ -9175,7 +8975,7 @@
         <v>4.26</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>20</v>
       </c>
@@ -9198,7 +8998,7 @@
         <v>3.72</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>18</v>
       </c>
@@ -9221,7 +9021,7 @@
         <v>3.84</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
@@ -9244,7 +9044,7 @@
         <v>3.73</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>19</v>
       </c>
@@ -9267,7 +9067,7 @@
         <v>4.26</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>18</v>
       </c>
@@ -9290,7 +9090,7 @@
         <v>3.84</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>20</v>
       </c>
@@ -9313,7 +9113,7 @@
         <v>3.73</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>19</v>
       </c>
@@ -9336,7 +9136,7 @@
         <v>4.26</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>18</v>
       </c>
@@ -9359,7 +9159,7 @@
         <v>3.84</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>20</v>
       </c>
@@ -9382,7 +9182,7 @@
         <v>3.74</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>19</v>
       </c>
@@ -9405,7 +9205,7 @@
         <v>4.2699999999999996</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>18</v>
       </c>
@@ -9428,7 +9228,7 @@
         <v>3.85</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>20</v>
       </c>
@@ -9451,7 +9251,7 @@
         <v>3.73</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>19</v>
       </c>
@@ -9474,7 +9274,7 @@
         <v>4.2699999999999996</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>18</v>
       </c>
@@ -9497,7 +9297,7 @@
         <v>3.85</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>20</v>
       </c>
@@ -9520,7 +9320,7 @@
         <v>3.72</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>19</v>
       </c>
@@ -9543,7 +9343,7 @@
         <v>4.2699999999999996</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>18</v>
       </c>
@@ -9566,7 +9366,7 @@
         <v>3.85</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>20</v>
       </c>
@@ -9589,7 +9389,7 @@
         <v>3.73</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>19</v>
       </c>
@@ -9612,7 +9412,7 @@
         <v>4.2699999999999996</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>18</v>
       </c>
@@ -9635,7 +9435,7 @@
         <v>3.85</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>20</v>
       </c>
@@ -9658,7 +9458,7 @@
         <v>3.72</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>19</v>
       </c>
@@ -9681,7 +9481,7 @@
         <v>4.2699999999999996</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>18</v>
       </c>
@@ -9704,7 +9504,7 @@
         <v>3.85</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>20</v>
       </c>
@@ -9727,7 +9527,7 @@
         <v>3.74</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>19</v>
       </c>
@@ -9750,7 +9550,7 @@
         <v>4.2699999999999996</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>18</v>
       </c>
@@ -9773,7 +9573,7 @@
         <v>3.85</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>20</v>
       </c>
@@ -9796,7 +9596,7 @@
         <v>3.74</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>19</v>
       </c>
@@ -9832,13 +9632,13 @@
       <selection activeCell="A3" sqref="A3:G32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -9856,7 +9656,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B2" s="4" t="s">
         <v>13</v>
       </c>
@@ -9882,7 +9682,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>18</v>
       </c>
@@ -9905,7 +9705,7 @@
         <v>3.83</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>18</v>
       </c>
@@ -9928,7 +9728,7 @@
         <v>3.84</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
@@ -9951,7 +9751,7 @@
         <v>3.84</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>18</v>
       </c>
@@ -9974,7 +9774,7 @@
         <v>3.84</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>18</v>
       </c>
@@ -9997,7 +9797,7 @@
         <v>3.85</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>18</v>
       </c>
@@ -10020,7 +9820,7 @@
         <v>3.85</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>18</v>
       </c>
@@ -10043,7 +9843,7 @@
         <v>3.85</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>18</v>
       </c>
@@ -10066,7 +9866,7 @@
         <v>3.85</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>18</v>
       </c>
@@ -10089,7 +9889,7 @@
         <v>3.85</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>18</v>
       </c>
@@ -10112,7 +9912,7 @@
         <v>3.85</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>20</v>
       </c>
@@ -10135,7 +9935,7 @@
         <v>3.72</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>20</v>
       </c>
@@ -10158,7 +9958,7 @@
         <v>3.73</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>20</v>
       </c>
@@ -10181,7 +9981,7 @@
         <v>3.73</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>20</v>
       </c>
@@ -10204,7 +10004,7 @@
         <v>3.74</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>20</v>
       </c>
@@ -10227,7 +10027,7 @@
         <v>3.73</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>20</v>
       </c>
@@ -10250,7 +10050,7 @@
         <v>3.72</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>20</v>
       </c>
@@ -10273,7 +10073,7 @@
         <v>3.73</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>20</v>
       </c>
@@ -10296,7 +10096,7 @@
         <v>3.72</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>20</v>
       </c>
@@ -10319,7 +10119,7 @@
         <v>3.74</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>20</v>
       </c>
@@ -10342,7 +10142,7 @@
         <v>3.74</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>19</v>
       </c>
@@ -10365,7 +10165,7 @@
         <v>4.26</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>19</v>
       </c>
@@ -10388,7 +10188,7 @@
         <v>4.26</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>19</v>
       </c>
@@ -10411,7 +10211,7 @@
         <v>4.26</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>19</v>
       </c>
@@ -10434,7 +10234,7 @@
         <v>4.2699999999999996</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>19</v>
       </c>
@@ -10457,7 +10257,7 @@
         <v>4.2699999999999996</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>19</v>
       </c>
@@ -10480,7 +10280,7 @@
         <v>4.2699999999999996</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>19</v>
       </c>
@@ -10503,7 +10303,7 @@
         <v>4.2699999999999996</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>19</v>
       </c>
@@ -10526,7 +10326,7 @@
         <v>4.2699999999999996</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>19</v>
       </c>
@@ -10549,7 +10349,7 @@
         <v>4.2699999999999996</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>19</v>
       </c>
@@ -10583,19 +10383,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I69"/>
+  <dimension ref="A1:T69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -10613,7 +10413,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B2" s="4" t="s">
         <v>13</v>
       </c>
@@ -10639,7 +10439,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>18</v>
       </c>
@@ -10662,7 +10462,7 @@
         <v>3.83</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
@@ -10685,7 +10485,7 @@
         <v>3.84</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>18</v>
       </c>
@@ -10708,7 +10508,7 @@
         <v>3.82</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>18</v>
       </c>
@@ -10731,7 +10531,7 @@
         <v>3.82</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>18</v>
       </c>
@@ -10754,7 +10554,7 @@
         <v>3.83</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>18</v>
       </c>
@@ -10777,7 +10577,7 @@
         <v>3.84</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>18</v>
       </c>
@@ -10800,7 +10600,7 @@
         <v>3.84</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>18</v>
       </c>
@@ -10823,7 +10623,7 @@
         <v>3.83</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>18</v>
       </c>
@@ -10846,7 +10646,7 @@
         <v>3.85</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>18</v>
       </c>
@@ -10869,7 +10669,7 @@
         <v>3.83</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>18</v>
       </c>
@@ -10892,7 +10692,7 @@
         <v>3.84</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>18</v>
       </c>
@@ -10915,7 +10715,7 @@
         <v>3.84</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>18</v>
       </c>
@@ -10938,7 +10738,7 @@
         <v>3.84</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>18</v>
       </c>
@@ -10961,7 +10761,7 @@
         <v>3.85</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>18</v>
       </c>
@@ -10984,7 +10784,7 @@
         <v>3.85</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>18</v>
       </c>
@@ -11007,7 +10807,7 @@
         <v>3.85</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>18</v>
       </c>
@@ -11030,7 +10830,7 @@
         <v>3.85</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>18</v>
       </c>
@@ -11052,8 +10852,26 @@
       <c r="G21" s="4">
         <v>3.85</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J21" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K21">
+        <v>4.6900000000000004</v>
+      </c>
+      <c r="L21">
+        <v>29</v>
+      </c>
+      <c r="M21">
+        <v>4.7389999999999999</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>16703</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>18</v>
       </c>
@@ -11075,8 +10893,29 @@
       <c r="G22" s="4">
         <v>3.85</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J22" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K22">
+        <v>4.68</v>
+      </c>
+      <c r="L22">
+        <v>48</v>
+      </c>
+      <c r="M22">
+        <v>7.1942399999999997</v>
+      </c>
+      <c r="N22">
+        <v>100</v>
+      </c>
+      <c r="O22">
+        <v>7172</v>
+      </c>
+      <c r="T22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>20</v>
       </c>
@@ -11098,8 +10937,26 @@
       <c r="G23" s="4">
         <v>4.26</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J23" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K23">
+        <v>4.68</v>
+      </c>
+      <c r="L23">
+        <v>47</v>
+      </c>
+      <c r="M23">
+        <v>7.4626999999999999</v>
+      </c>
+      <c r="N23">
+        <v>100</v>
+      </c>
+      <c r="O23">
+        <v>7426</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>20</v>
       </c>
@@ -11121,8 +10978,26 @@
       <c r="G24" s="4">
         <v>3.71</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J24" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K24">
+        <v>4.67</v>
+      </c>
+      <c r="L24">
+        <v>17</v>
+      </c>
+      <c r="M24">
+        <v>4.0816299999999996</v>
+      </c>
+      <c r="N24">
+        <v>100</v>
+      </c>
+      <c r="O24">
+        <v>6346</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>20</v>
       </c>
@@ -11145,7 +11020,7 @@
         <v>3.72</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>20</v>
       </c>
@@ -11168,7 +11043,7 @@
         <v>3.72</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>20</v>
       </c>
@@ -11191,7 +11066,7 @@
         <v>3.72</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>20</v>
       </c>
@@ -11214,7 +11089,7 @@
         <v>3.72</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>20</v>
       </c>
@@ -11237,7 +11112,7 @@
         <v>3.72</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>20</v>
       </c>
@@ -11260,7 +11135,7 @@
         <v>3.72</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>20</v>
       </c>
@@ -11283,7 +11158,7 @@
         <v>3.73</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>20</v>
       </c>
@@ -11306,7 +11181,7 @@
         <v>3.72</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>20</v>
       </c>
@@ -11329,7 +11204,7 @@
         <v>3.73</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>20</v>
       </c>
@@ -11352,7 +11227,7 @@
         <v>3.73</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>20</v>
       </c>
@@ -11375,7 +11250,7 @@
         <v>3.74</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>20</v>
       </c>
@@ -11398,7 +11273,7 @@
         <v>3.73</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>20</v>
       </c>
@@ -11421,7 +11296,7 @@
         <v>3.72</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>20</v>
       </c>
@@ -11444,7 +11319,7 @@
         <v>3.73</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>20</v>
       </c>
@@ -11467,7 +11342,7 @@
         <v>3.72</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>20</v>
       </c>
@@ -11490,7 +11365,7 @@
         <v>3.74</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>20</v>
       </c>
@@ -11513,7 +11388,7 @@
         <v>3.74</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>19</v>
       </c>
@@ -11536,7 +11411,7 @@
         <v>3.74</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>19</v>
       </c>
@@ -11559,7 +11434,7 @@
         <v>4.2699999999999996</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>19</v>
       </c>
@@ -11582,7 +11457,7 @@
         <v>4.2699999999999996</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>19</v>
       </c>
@@ -11605,7 +11480,7 @@
         <v>4.26</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>19</v>
       </c>
@@ -11628,7 +11503,7 @@
         <v>4.26</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>19</v>
       </c>
@@ -11651,7 +11526,7 @@
         <v>4.26</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>19</v>
       </c>
@@ -11674,7 +11549,7 @@
         <v>4.26</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
         <v>19</v>
       </c>
@@ -11697,7 +11572,7 @@
         <v>4.3600000000000003</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>19</v>
       </c>
@@ -11720,7 +11595,7 @@
         <v>4.26</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
         <v>19</v>
       </c>
@@ -11743,7 +11618,7 @@
         <v>4.26</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>19</v>
       </c>
@@ -11766,7 +11641,7 @@
         <v>4.26</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>19</v>
       </c>
@@ -11789,7 +11664,7 @@
         <v>4.26</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
         <v>19</v>
       </c>
@@ -11812,7 +11687,7 @@
         <v>4.2699999999999996</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
         <v>19</v>
       </c>
@@ -11835,7 +11710,7 @@
         <v>4.2699999999999996</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
         <v>19</v>
       </c>
@@ -11858,7 +11733,7 @@
         <v>4.2699999999999996</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
         <v>19</v>
       </c>
@@ -11881,7 +11756,7 @@
         <v>4.2699999999999996</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
         <v>19</v>
       </c>
@@ -11904,7 +11779,7 @@
         <v>4.2699999999999996</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
         <v>19</v>
       </c>
@@ -11927,7 +11802,7 @@
         <v>4.2699999999999996</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
         <v>19</v>
       </c>
@@ -11950,7 +11825,7 @@
         <v>4.2699999999999996</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>12</v>
       </c>
@@ -11973,7 +11848,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>12</v>
       </c>
@@ -11996,7 +11871,7 @@
         <v>4.0199999999999996</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>12</v>
       </c>
@@ -12019,7 +11894,7 @@
         <v>4.0199999999999996</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>12</v>
       </c>
@@ -12042,7 +11917,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>12</v>
       </c>
@@ -12065,7 +11940,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>12</v>
       </c>
@@ -12088,7 +11963,7 @@
         <v>4.01</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>12</v>
       </c>
@@ -12111,7 +11986,7 @@
         <v>3.99</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>12</v>
       </c>
@@ -12134,7 +12009,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>12</v>
       </c>

</xml_diff>